<commit_message>
Corrected minor mistake in excel file.
</commit_message>
<xml_diff>
--- a/Predavanje_00/data_raw/odsotnosti_R.xlsx
+++ b/Predavanje_00/data_raw/odsotnosti_R.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Gregor\Documents\shared_files\workshops\R-za-neprogramerje\Predavanje_00\data_raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF29B168-AEB8-4364-9EDF-F039BEF9C485}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21AA785D-8F17-47C2-8119-CA8D04EE3822}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9060" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Odsotnosti" sheetId="2" r:id="rId1"/>
@@ -512,8 +512,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C683"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N11" sqref="N11"/>
+    <sheetView topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8037,8 +8037,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B29"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8080,7 +8080,6 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A5">
-        <f>A4 + 1</f>
         <v>4</v>
       </c>
       <c r="B5" t="s">
@@ -8089,7 +8088,6 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A6">
-        <f t="shared" ref="A6:A28" si="0">A5 + 1</f>
         <v>5</v>
       </c>
       <c r="B6" t="s">
@@ -8098,7 +8096,6 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A7">
-        <f t="shared" si="0"/>
         <v>6</v>
       </c>
       <c r="B7" t="s">
@@ -8107,7 +8104,6 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A8">
-        <f t="shared" si="0"/>
         <v>7</v>
       </c>
       <c r="B8" t="s">
@@ -8116,7 +8112,6 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A9">
-        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="B9" t="s">
@@ -8125,7 +8120,6 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A10">
-        <f t="shared" si="0"/>
         <v>9</v>
       </c>
       <c r="B10" t="s">
@@ -8134,7 +8128,6 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A11">
-        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="B11" t="s">
@@ -8143,7 +8136,6 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A12">
-        <f t="shared" si="0"/>
         <v>11</v>
       </c>
       <c r="B12" t="s">
@@ -8152,7 +8144,6 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A13">
-        <f t="shared" si="0"/>
         <v>12</v>
       </c>
       <c r="B13" t="s">
@@ -8161,7 +8152,6 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A14">
-        <f t="shared" si="0"/>
         <v>13</v>
       </c>
       <c r="B14" t="s">
@@ -8170,7 +8160,6 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A15">
-        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="B15" t="s">
@@ -8179,7 +8168,6 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A16">
-        <f t="shared" si="0"/>
         <v>15</v>
       </c>
       <c r="B16" t="s">
@@ -8188,7 +8176,6 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A17">
-        <f t="shared" si="0"/>
         <v>16</v>
       </c>
       <c r="B17" t="s">
@@ -8197,7 +8184,6 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A18">
-        <f t="shared" si="0"/>
         <v>17</v>
       </c>
       <c r="B18" t="s">
@@ -8206,7 +8192,6 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A19">
-        <f t="shared" si="0"/>
         <v>18</v>
       </c>
       <c r="B19" t="s">
@@ -8215,7 +8200,6 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A20">
-        <f t="shared" si="0"/>
         <v>19</v>
       </c>
       <c r="B20" t="s">
@@ -8224,7 +8208,6 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A21">
-        <f t="shared" si="0"/>
         <v>20</v>
       </c>
       <c r="B21" t="s">
@@ -8233,7 +8216,6 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A22">
-        <f t="shared" si="0"/>
         <v>21</v>
       </c>
       <c r="B22" t="s">
@@ -8242,7 +8224,6 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A23">
-        <f t="shared" si="0"/>
         <v>22</v>
       </c>
       <c r="B23" t="s">
@@ -8251,7 +8232,6 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A24">
-        <f t="shared" si="0"/>
         <v>23</v>
       </c>
       <c r="B24" t="s">
@@ -8260,7 +8240,6 @@
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A25">
-        <f t="shared" si="0"/>
         <v>24</v>
       </c>
       <c r="B25" t="s">
@@ -8269,7 +8248,6 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A26">
-        <f t="shared" si="0"/>
         <v>25</v>
       </c>
       <c r="B26" t="s">
@@ -8278,7 +8256,6 @@
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A27">
-        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="B27" t="s">
@@ -8287,7 +8264,6 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A28">
-        <f t="shared" si="0"/>
         <v>27</v>
       </c>
       <c r="B28" t="s">

</xml_diff>